<commit_message>
ImportExport: Excel Starting List aligned with DFPCreator
</commit_message>
<xml_diff>
--- a/AirNavigationRaceLive/Resources/Template.xlsx
+++ b/AirNavigationRaceLive/Resources/Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\VS2015\Anrl\anrl\AirNavigationRaceLive\AirNavigationRaceLive\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zugerarm1\source\repos\ANR_Scoring_And_Visualisation\AirNavigationRaceLive\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21486" windowHeight="7290" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21490" windowHeight="7290" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Participants" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Lastname</t>
   </si>
@@ -58,37 +58,25 @@
     <t>Take Off</t>
   </si>
   <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>End</t>
-  </si>
-  <si>
     <t>Route</t>
   </si>
   <si>
-    <t>Mögliche Routen</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>Lastname + Firstname</t>
   </si>
   <si>
-    <t>CNumber</t>
-  </si>
-  <si>
-    <t>Datum</t>
+    <t>Start Planning</t>
+  </si>
+  <si>
+    <t>End Planning</t>
+  </si>
+  <si>
+    <t>SP Gate</t>
+  </si>
+  <si>
+    <t>FP Gate</t>
+  </si>
+  <si>
+    <t>Crew ID</t>
   </si>
 </sst>
 </file>
@@ -135,16 +123,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -160,7 +146,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -428,14 +414,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.83984375" customWidth="1"/>
-    <col min="2" max="2" width="16.578125" customWidth="1"/>
-    <col min="3" max="3" width="44.3671875" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="44.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,868 +429,868 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C2" t="str">
         <f>CONCATENATE(A2," ",B2)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C3" t="str">
         <f t="shared" ref="C3:C66" si="0">CONCATENATE(A3," ",B3)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C4" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C5" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C6" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C21" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C27" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C29" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C30" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C31" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C32" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C35" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C36" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C37" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C38" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C40" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C41" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C42" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C44" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C45" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C46" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C47" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C48" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C49" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C50" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C51" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C52" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C53" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C54" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C55" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C56" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C57" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C58" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C59" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C60" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C61" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C62" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C63" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C64" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C65" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C66" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C67" t="str">
         <f t="shared" ref="C67:C130" si="1">CONCATENATE(A67," ",B67)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C68" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C69" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C70" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C71" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C72" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C73" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C74" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C75" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C76" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C77" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C78" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C79" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C80" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C81" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C82" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C83" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C84" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C85" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C86" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C87" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C88" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C89" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C90" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C91" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C92" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C93" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C94" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C95" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C96" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C97" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C98" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C99" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C100" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C101" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C102" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C103" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C104" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C105" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C106" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C107" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C108" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C109" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C110" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C111" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C112" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C113" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C114" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C115" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C116" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C117" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C118" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C119" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C120" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C121" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C122" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C123" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C124" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C125" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C126" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C127" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C128" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C129" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C130" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C131" t="str">
         <f t="shared" ref="C131:C145" si="2">CONCATENATE(A131," ",B131)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C132" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C133" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C134" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C135" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C136" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C137" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C138" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C139" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C140" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C141" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C142" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C143" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C144" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C145" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
@@ -1324,14 +1310,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.26171875" customWidth="1"/>
-    <col min="3" max="3" width="33.68359375" customWidth="1"/>
-    <col min="4" max="4" width="40.05078125" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="33.6328125" customWidth="1"/>
+    <col min="4" max="4" width="40.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1367,30 +1353,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.89453125" customWidth="1"/>
-    <col min="2" max="2" width="9.5234375" customWidth="1"/>
-    <col min="3" max="3" width="13.47265625" customWidth="1"/>
-    <col min="4" max="4" width="44.26171875" customWidth="1"/>
-    <col min="5" max="5" width="12.1015625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.734375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.62890625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.20703125" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="44.26953125" customWidth="1"/>
+    <col min="5" max="6" width="19.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.7265625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.6328125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="6.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
@@ -1398,53 +1385,32 @@
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="J2" s="3"/>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="K3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="K4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="K5" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="A2:H100" name="StartListe"/>
+    <protectedRange sqref="A2:J100" name="StartListe"/>
   </protectedRanges>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H100">
-      <formula1>$K$2:$K$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J100">
+      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>